<commit_message>
Pinouts correct last version.
</commit_message>
<xml_diff>
--- a/Hardware/InOuts SiDi.xlsx
+++ b/Hardware/InOuts SiDi.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCAC222E-067B-4D51-8955-EDDC61A3BFA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6ED5C23-3351-4D2C-BA7D-097B4F15AA73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -274,9 +274,6 @@
     <t>PIN_C11</t>
   </si>
   <si>
-    <t>PIN_D11</t>
-  </si>
-  <si>
     <t>PIN_A2</t>
   </si>
   <si>
@@ -458,6 +455,9 @@
   </si>
   <si>
     <t>PIN_C2</t>
+  </si>
+  <si>
+    <t>PIN_R4</t>
   </si>
 </sst>
 </file>
@@ -929,8 +929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A5:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -957,7 +957,7 @@
         <v>69</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -968,10 +968,10 @@
         <v>79</v>
       </c>
       <c r="D6" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="E6" s="23" t="s">
         <v>133</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -979,13 +979,13 @@
         <v>15</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D7" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" s="12" t="s">
         <v>107</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -993,13 +993,13 @@
         <v>14</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -1007,13 +1007,13 @@
         <v>13</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>1</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -1027,7 +1027,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -1035,13 +1035,13 @@
         <v>11</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>3</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -1055,7 +1055,7 @@
         <v>4</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -1077,7 +1077,7 @@
         <v>8</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>45</v>
@@ -1105,13 +1105,13 @@
         <v>6</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>47</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -1125,15 +1125,15 @@
         <v>48</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D18" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="E18" s="8" t="s">
         <v>137</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -1141,7 +1141,7 @@
         <v>49</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -1149,7 +1149,7 @@
         <v>50</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -1159,7 +1159,7 @@
         <v>51</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -1173,7 +1173,7 @@
         <v>52</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -1187,7 +1187,7 @@
         <v>53</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -1201,7 +1201,7 @@
         <v>54</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -1209,13 +1209,13 @@
         <v>21</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>77</v>
+        <v>145</v>
       </c>
       <c r="D25" s="17" t="s">
         <v>55</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -1223,13 +1223,13 @@
         <v>22</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D26" s="17" t="s">
         <v>56</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -1237,13 +1237,13 @@
         <v>23</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D27" s="17" t="s">
         <v>57</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
@@ -1251,13 +1251,13 @@
         <v>24</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D28" s="17" t="s">
         <v>58</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -1265,13 +1265,13 @@
         <v>25</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D29" s="17" t="s">
         <v>59</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
@@ -1279,13 +1279,13 @@
         <v>26</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D30" s="17" t="s">
         <v>60</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
@@ -1293,13 +1293,13 @@
         <v>27</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D31" s="19" t="s">
         <v>62</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
@@ -1307,13 +1307,13 @@
         <v>28</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D32" s="19" t="s">
         <v>63</v>
       </c>
       <c r="E32" s="20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
@@ -1321,13 +1321,13 @@
         <v>29</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D33" s="19" t="s">
         <v>64</v>
       </c>
       <c r="E33" s="20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
@@ -1335,13 +1335,13 @@
         <v>30</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D34" s="19" t="s">
         <v>65</v>
       </c>
       <c r="E34" s="20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
@@ -1349,13 +1349,13 @@
         <v>31</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D35" s="19" t="s">
         <v>66</v>
       </c>
       <c r="E35" s="20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
@@ -1363,13 +1363,13 @@
         <v>32</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D36" s="19" t="s">
         <v>67</v>
       </c>
       <c r="E36" s="20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
@@ -1377,13 +1377,13 @@
         <v>33</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D37" s="21" t="s">
         <v>68</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
@@ -1391,13 +1391,13 @@
         <v>34</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D38" s="21" t="s">
         <v>61</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
@@ -1405,7 +1405,7 @@
         <v>35</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
@@ -1413,7 +1413,7 @@
         <v>36</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
@@ -1421,7 +1421,7 @@
         <v>37</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
@@ -1429,7 +1429,7 @@
         <v>38</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
@@ -1437,7 +1437,7 @@
         <v>39</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
@@ -1445,7 +1445,7 @@
         <v>40</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
@@ -1453,7 +1453,7 @@
         <v>41</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
@@ -1461,7 +1461,7 @@
         <v>42</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
@@ -1469,7 +1469,7 @@
         <v>43</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>